<commit_message>
ka cs pie 1-7
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-1.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,10 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1075,9 +1079,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D1:H21"/>
+  <dimension ref="D1:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -1143,9 +1147,14 @@
     <row r="16" spans="4:6">
       <c r="D16" s="5"/>
     </row>
-    <row r="21" spans="8:8">
+    <row r="21" spans="8:9">
       <c r="H21" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9">
+      <c r="I23" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1162,7 +1171,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>

</xml_diff>